<commit_message>
Added methods for productRepositoryInDB
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="0" windowWidth="24360" windowHeight="17120"/>
+    <workbookView xWindow="2860" yWindow="0" windowWidth="24360" windowHeight="17120"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -880,6 +880,9 @@
                 <c:pt idx="9">
                   <c:v>115.0</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>69.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -971,11 +974,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111210520"/>
-        <c:axId val="2111213496"/>
+        <c:axId val="2118237896"/>
+        <c:axId val="2118234904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111210520"/>
+        <c:axId val="2118237896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,7 +987,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111213496"/>
+        <c:crossAx val="2118234904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -992,7 +995,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111213496"/>
+        <c:axId val="2118234904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111210520"/>
+        <c:crossAx val="2118237896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1356,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1517,7 +1520,9 @@
       <c r="L5" s="4">
         <v>0</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -1566,7 +1571,9 @@
       <c r="L6" s="4">
         <v>0</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -1615,7 +1622,9 @@
       <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -1664,7 +1673,9 @@
       <c r="L8" s="4">
         <v>0</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -1713,7 +1724,9 @@
       <c r="L9" s="4">
         <v>0</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -1762,7 +1775,9 @@
       <c r="L10" s="4">
         <v>0</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
@@ -1811,7 +1826,9 @@
       <c r="L11" s="4">
         <v>0</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -1860,7 +1877,9 @@
       <c r="L12" s="4">
         <v>0</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -1909,7 +1928,9 @@
       <c r="L13" s="4">
         <v>0</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -1958,7 +1979,9 @@
       <c r="L14" s="4">
         <v>0</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
@@ -2007,7 +2030,9 @@
       <c r="L15" s="4">
         <v>0</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
@@ -2056,7 +2081,9 @@
       <c r="L16" s="4">
         <v>0</v>
       </c>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -2105,7 +2132,9 @@
       <c r="L17" s="4">
         <v>0</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -2154,7 +2183,9 @@
       <c r="L18" s="4">
         <v>21</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -2203,7 +2234,9 @@
       <c r="L19" s="4">
         <v>0</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -2252,7 +2285,9 @@
       <c r="L20" s="4">
         <v>8</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4">
+        <v>3</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -2301,7 +2336,9 @@
       <c r="L21" s="4">
         <v>8</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4">
+        <v>3</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -2350,7 +2387,9 @@
       <c r="L22" s="4">
         <v>5</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2399,7 +2438,9 @@
       <c r="L23" s="4">
         <v>8</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4">
+        <v>3</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2448,7 +2489,9 @@
       <c r="L24" s="4">
         <v>40</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4">
+        <v>35</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -2497,7 +2540,9 @@
       <c r="L25" s="4">
         <v>15</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4">
+        <v>15</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -2546,7 +2591,9 @@
       <c r="L26" s="4">
         <v>10</v>
       </c>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4">
+        <v>10</v>
+      </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -2654,7 +2701,10 @@
         <f>SUM(L5:L26)</f>
         <v>115</v>
       </c>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4">
+        <f>SUM(M5:M27)</f>
+        <v>69</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>

</xml_diff>

<commit_message>
tested code in cartRepo, userRepo, categoryRepo product repo to gooo
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -678,7 +678,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -699,6 +699,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -777,7 +779,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -800,8 +802,10 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -882,6 +886,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,11 +981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118237896"/>
-        <c:axId val="2118234904"/>
+        <c:axId val="2033070088"/>
+        <c:axId val="2033073064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2118237896"/>
+        <c:axId val="2033070088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -987,7 +994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118234904"/>
+        <c:crossAx val="2033073064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -995,7 +1002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118234904"/>
+        <c:axId val="2033073064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1006,7 +1013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118237896"/>
+        <c:crossAx val="2033070088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1359,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1523,7 +1530,9 @@
       <c r="M5" s="4">
         <v>0</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -1574,7 +1583,9 @@
       <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -1625,7 +1636,9 @@
       <c r="M7" s="4">
         <v>0</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1676,7 +1689,9 @@
       <c r="M8" s="4">
         <v>0</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -1727,7 +1742,9 @@
       <c r="M9" s="4">
         <v>0</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1778,7 +1795,9 @@
       <c r="M10" s="4">
         <v>0</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1829,7 +1848,9 @@
       <c r="M11" s="4">
         <v>0</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1880,7 +1901,9 @@
       <c r="M12" s="4">
         <v>0</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -1931,7 +1954,9 @@
       <c r="M13" s="4">
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -1982,7 +2007,9 @@
       <c r="M14" s="4">
         <v>0</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -2033,7 +2060,9 @@
       <c r="M15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -2084,7 +2113,9 @@
       <c r="M16" s="4">
         <v>0</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -2135,7 +2166,9 @@
       <c r="M17" s="4">
         <v>0</v>
       </c>
-      <c r="N17" s="4"/>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -2186,7 +2219,9 @@
       <c r="M18" s="4">
         <v>0</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -2237,7 +2272,9 @@
       <c r="M19" s="4">
         <v>0</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -2288,7 +2325,9 @@
       <c r="M20" s="4">
         <v>3</v>
       </c>
-      <c r="N20" s="4"/>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -2339,7 +2378,9 @@
       <c r="M21" s="4">
         <v>3</v>
       </c>
-      <c r="N21" s="4"/>
+      <c r="N21" s="4">
+        <v>1</v>
+      </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
@@ -2390,7 +2431,9 @@
       <c r="M22" s="4">
         <v>0</v>
       </c>
-      <c r="N22" s="4"/>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2441,7 +2484,9 @@
       <c r="M23" s="4">
         <v>3</v>
       </c>
-      <c r="N23" s="4"/>
+      <c r="N23" s="4">
+        <v>1</v>
+      </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -2492,7 +2537,9 @@
       <c r="M24" s="4">
         <v>35</v>
       </c>
-      <c r="N24" s="4"/>
+      <c r="N24" s="4">
+        <v>30</v>
+      </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
@@ -2543,7 +2590,9 @@
       <c r="M25" s="4">
         <v>15</v>
       </c>
-      <c r="N25" s="4"/>
+      <c r="N25" s="4">
+        <v>15</v>
+      </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -2594,7 +2643,9 @@
       <c r="M26" s="4">
         <v>10</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" s="4">
+        <v>10</v>
+      </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
@@ -2705,7 +2756,10 @@
         <f>SUM(M5:M27)</f>
         <v>69</v>
       </c>
-      <c r="N29" s="4"/>
+      <c r="N29" s="4">
+        <f>SUM(N5:N27)</f>
+        <v>58</v>
+      </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>

</xml_diff>

<commit_message>
Added test-class for presentation fridat 31th
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -678,7 +678,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -699,6 +699,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -779,7 +785,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -803,9 +809,15 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,10 +846,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0938435235436208"/>
-          <c:y val="0.0694443265907134"/>
-          <c:w val="0.669448926613311"/>
-          <c:h val="0.822469378827647"/>
+          <c:x val="0.0454217258005699"/>
+          <c:y val="0.047682119205298"/>
+          <c:w val="0.80482421901379"/>
+          <c:h val="0.898419565104031"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -846,49 +858,44 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ADI-burndown'!$B$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>'ADI-burndown'!$C$29:$Z$29</c:f>
+              <c:f>'ADI-burndown'!$F$29:$Z$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>214.0</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>202.0</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>202.0</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189.0</c:v>
+                  <c:v>155.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>168.0</c:v>
+                  <c:v>140.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>168.0</c:v>
+                  <c:v>94.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.0</c:v>
+                  <c:v>83.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>58.0</c:v>
+                  <c:v>70.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,72 +905,61 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'ADI-burndown'!$B$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>'ADI-burndown'!$C$30:$Z$30</c:f>
+              <c:f>'ADI-burndown'!$F$30:$Z$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="3">
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
                   <c:v>240.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="1">
                   <c:v>225.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="2">
                   <c:v>210.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="3">
                   <c:v>195.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="4">
                   <c:v>180.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="5">
                   <c:v>165.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="6">
                   <c:v>150.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="7">
                   <c:v>135.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="8">
                   <c:v>120.0</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="9">
                   <c:v>105.0</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="10">
                   <c:v>90.0</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="11">
                   <c:v>75.0</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="12">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="13">
                   <c:v>45.0</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="14">
                   <c:v>30.0</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="15">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="16">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -981,11 +977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2033070088"/>
-        <c:axId val="2033073064"/>
+        <c:axId val="2112537208"/>
+        <c:axId val="2112541944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2033070088"/>
+        <c:axId val="2112537208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2033073064"/>
+        <c:crossAx val="2112541944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2033073064"/>
+        <c:axId val="2112541944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,23 +1009,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2033070088"/>
+        <c:crossAx val="2112537208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.83034921421416"/>
-          <c:y val="0.0699393221008664"/>
-          <c:w val="0.139982334629512"/>
-          <c:h val="0.0959756912106417"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1048,20 +1035,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1366,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1533,8 +1520,12 @@
       <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
@@ -1586,8 +1577,12 @@
       <c r="N6" s="4">
         <v>0</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -1639,8 +1634,12 @@
       <c r="N7" s="4">
         <v>0</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1692,8 +1691,12 @@
       <c r="N8" s="4">
         <v>0</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1745,8 +1748,12 @@
       <c r="N9" s="4">
         <v>0</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1798,8 +1805,12 @@
       <c r="N10" s="4">
         <v>0</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
@@ -1851,8 +1862,12 @@
       <c r="N11" s="4">
         <v>0</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1904,8 +1919,12 @@
       <c r="N12" s="4">
         <v>0</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1957,8 +1976,12 @@
       <c r="N13" s="4">
         <v>0</v>
       </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -2010,8 +2033,12 @@
       <c r="N14" s="4">
         <v>0</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -2063,8 +2090,12 @@
       <c r="N15" s="4">
         <v>0</v>
       </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
@@ -2116,8 +2147,12 @@
       <c r="N16" s="4">
         <v>0</v>
       </c>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
@@ -2169,8 +2204,12 @@
       <c r="N17" s="4">
         <v>0</v>
       </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -2222,8 +2261,12 @@
       <c r="N18" s="4">
         <v>0</v>
       </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -2275,8 +2318,12 @@
       <c r="N19" s="4">
         <v>0</v>
       </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
@@ -2328,8 +2375,12 @@
       <c r="N20" s="4">
         <v>1</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
@@ -2381,8 +2432,12 @@
       <c r="N21" s="4">
         <v>1</v>
       </c>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -2434,8 +2489,12 @@
       <c r="N22" s="4">
         <v>0</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
@@ -2487,8 +2546,12 @@
       <c r="N23" s="4">
         <v>1</v>
       </c>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
@@ -2540,8 +2603,12 @@
       <c r="N24" s="4">
         <v>30</v>
       </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="O24" s="4">
+        <v>20</v>
+      </c>
+      <c r="P24" s="4">
+        <v>20</v>
+      </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
@@ -2567,34 +2634,38 @@
         <v>106</v>
       </c>
       <c r="F25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M25" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="N25" s="4">
-        <v>15</v>
-      </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="O25" s="4">
+        <v>30</v>
+      </c>
+      <c r="P25" s="4">
+        <v>30</v>
+      </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
@@ -2620,34 +2691,38 @@
         <v>107</v>
       </c>
       <c r="F26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M26" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N26" s="4">
-        <v>10</v>
-      </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="O26" s="4">
+        <v>20</v>
+      </c>
+      <c r="P26" s="4">
+        <v>20</v>
+      </c>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
@@ -2726,42 +2801,48 @@
       <c r="E29" s="5"/>
       <c r="F29" s="4">
         <f>SUM(F5:F28)</f>
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="G29" s="4">
         <f>SUM(G5:G26)</f>
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="H29" s="4">
         <f>SUM(H5:H28)</f>
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="I29" s="4">
         <f>SUM(I5:I28)</f>
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="J29" s="4">
         <f>SUM(J5:J27)</f>
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="K29" s="4">
         <f>SUM(K5:K27)</f>
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="L29" s="4">
         <f>SUM(L5:L26)</f>
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="M29" s="4">
         <f>SUM(M5:M27)</f>
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="N29" s="4">
         <f>SUM(N5:N27)</f>
-        <v>58</v>
-      </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="O29" s="4">
+        <f>SUM(O6:O27)</f>
+        <v>70</v>
+      </c>
+      <c r="P29" s="4">
+        <f>SUM(P5:P27)</f>
+        <v>70</v>
+      </c>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
@@ -3226,6 +3307,7 @@
     <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added protocol from Scrum retrospective meeting
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="0" windowWidth="24360" windowHeight="17120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27380" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -977,11 +977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2112537208"/>
-        <c:axId val="2112541944"/>
+        <c:axId val="2094721368"/>
+        <c:axId val="2094724344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2112537208"/>
+        <c:axId val="2094721368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112541944"/>
+        <c:crossAx val="2094724344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112541944"/>
+        <c:axId val="2094724344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112537208"/>
+        <c:crossAx val="2094721368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1353,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3307,7 +3307,6 @@
     <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
added effective IDE usage from Jfokus
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27380" windowHeight="13020"/>
+    <workbookView xWindow="500" yWindow="4660" windowWidth="27380" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -977,11 +977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2094721368"/>
-        <c:axId val="2094724344"/>
+        <c:axId val="2067934808"/>
+        <c:axId val="2067937832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2094721368"/>
+        <c:axId val="2067934808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094724344"/>
+        <c:crossAx val="2067937832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2094724344"/>
+        <c:axId val="2067937832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2094721368"/>
+        <c:crossAx val="2067934808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1353,7 +1353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Began the console tool for out API
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
+    <workbookView minimized="1" xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -878,14 +878,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1105,11 +1105,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2085719976"/>
-        <c:axId val="2085722952"/>
+        <c:axId val="2083358984"/>
+        <c:axId val="2083361960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2085719976"/>
+        <c:axId val="2083358984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085722952"/>
+        <c:crossAx val="2083361960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085722952"/>
+        <c:axId val="2083361960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,14 +1137,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085719976"/>
+        <c:crossAx val="2083358984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1287,11 +1286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092128216"/>
-        <c:axId val="2092132264"/>
+        <c:axId val="2083452392"/>
+        <c:axId val="2083455368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2092128216"/>
+        <c:axId val="2083452392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092132264"/>
+        <c:crossAx val="2083455368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1308,7 +1307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092132264"/>
+        <c:axId val="2083455368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,14 +1318,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092128216"/>
+        <c:crossAx val="2083452392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1429,11 +1427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2095461000"/>
-        <c:axId val="2095462408"/>
+        <c:axId val="2083491640"/>
+        <c:axId val="2083494616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2095461000"/>
+        <c:axId val="2083491640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +1440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095462408"/>
+        <c:crossAx val="2083494616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1450,7 +1448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095462408"/>
+        <c:axId val="2083494616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1461,7 +1459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095461000"/>
+        <c:crossAx val="2083491640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3542,7 +3540,7 @@
       <c r="Z24" s="4">
         <v>0</v>
       </c>
-      <c r="AA24" s="37"/>
+      <c r="AA24" s="36"/>
     </row>
     <row r="25" spans="2:27">
       <c r="B25" s="3" t="s">
@@ -4469,11 +4467,11 @@
       </c>
     </row>
     <row r="37" spans="2:26">
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="5"/>
       <c r="F37" s="4">
         <f t="shared" ref="F37:P37" si="0">SUM(F5:F36)</f>
@@ -4531,11 +4529,11 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38" spans="2:26">
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="5"/>
       <c r="F38" s="4">
         <v>240</v>
@@ -4983,7 +4981,6 @@
     <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6447,97 +6444,97 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="35"/>
       <c r="E23" s="4">
-        <f>SUM(E3:E22)</f>
+        <f t="shared" ref="E23:O23" si="0">SUM(E3:E22)</f>
         <v>167</v>
       </c>
       <c r="F23" s="4">
-        <f>SUM(F3:F22)</f>
+        <f t="shared" si="0"/>
         <v>167</v>
       </c>
       <c r="G23" s="4">
-        <f>SUM(G3:G22)</f>
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="H23" s="4">
-        <f>SUM(H3:H22)</f>
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="I23" s="4">
-        <f>SUM(I3:I22)</f>
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="J23" s="4">
-        <f>SUM(J3:J22)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="K23" s="4">
-        <f>SUM(K3:K22)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="L23" s="4">
-        <f>SUM(L3:L22)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="M23" s="4">
-        <f>SUM(M3:M22)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="N23" s="4">
-        <f>SUM(N3:N22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O23" s="4">
-        <f>SUM(O3:O22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="35"/>
       <c r="E24" s="4">
         <v>120</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" ref="F24:O24" si="0">E24-15</f>
+        <f t="shared" ref="F24:M24" si="1">E24-15</f>
         <v>105</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="L24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N24" s="4"/>
@@ -6563,7 +6560,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6577,7 +6574,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="38"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="33" t="s">
         <v>62</v>
       </c>
@@ -7203,11 +7200,11 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="35"/>
       <c r="E15" s="4">
         <f>SUM(E3:E14)</f>
@@ -7225,45 +7222,45 @@
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="35"/>
       <c r="E16" s="4">
         <v>120</v>
       </c>
       <c r="F16" s="4">
-        <f>E16-15</f>
+        <f t="shared" ref="F16:M16" si="0">E16-15</f>
         <v>105</v>
       </c>
       <c r="G16" s="4">
-        <f>F16-15</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="H16" s="4">
-        <f>G16-15</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I16" s="4">
-        <f>H16-15</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="J16" s="4">
-        <f>I16-15</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="K16" s="4">
-        <f>J16-15</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="L16" s="4">
-        <f>K16-15</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M16" s="4">
-        <f>L16-15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" s="19"/>
@@ -7275,7 +7272,6 @@
     <mergeCell ref="A16:C16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Started createUser in consoleTool
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -1105,11 +1105,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083358984"/>
-        <c:axId val="2083361960"/>
+        <c:axId val="2079918664"/>
+        <c:axId val="2079921688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083358984"/>
+        <c:axId val="2079918664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1118,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083361960"/>
+        <c:crossAx val="2079921688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083361960"/>
+        <c:axId val="2079921688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,13 +1137,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083358984"/>
+        <c:crossAx val="2079918664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1286,11 +1287,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083452392"/>
-        <c:axId val="2083455368"/>
+        <c:axId val="2098868424"/>
+        <c:axId val="2098871400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083452392"/>
+        <c:axId val="2098868424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083455368"/>
+        <c:crossAx val="2098871400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1307,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083455368"/>
+        <c:axId val="2098871400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1318,13 +1319,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083452392"/>
+        <c:crossAx val="2098868424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1427,11 +1429,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083491640"/>
-        <c:axId val="2083494616"/>
+        <c:axId val="2099484664"/>
+        <c:axId val="2099487640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083491640"/>
+        <c:axId val="2099484664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083494616"/>
+        <c:crossAx val="2099487640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1448,7 +1450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083494616"/>
+        <c:axId val="2099487640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083491640"/>
+        <c:crossAx val="2099484664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5427,7 +5429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -6560,7 +6562,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Categories in DB changed to ENUM
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="142">
   <si>
     <t>Project</t>
   </si>
@@ -427,6 +427,36 @@
   </si>
   <si>
     <t>Ändra i API från boolean till Enum</t>
+  </si>
+  <si>
+    <t>Task 5.2</t>
+  </si>
+  <si>
+    <t>Task 5.3</t>
+  </si>
+  <si>
+    <t>Task 5.4</t>
+  </si>
+  <si>
+    <t>Task 5.6</t>
+  </si>
+  <si>
+    <t>Task 5.7</t>
+  </si>
+  <si>
+    <t>Revidering av coden API från boolean till Enum</t>
+  </si>
+  <si>
+    <t>Ändra User API</t>
+  </si>
+  <si>
+    <t>Ändra Category API</t>
+  </si>
+  <si>
+    <t>Ändra Cart Api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ändra Product API </t>
   </si>
 </sst>
 </file>
@@ -757,7 +787,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -778,6 +808,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -904,7 +954,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -946,6 +996,16 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
@@ -967,6 +1027,16 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1353,6 +1423,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1392,18 +1463,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$E$16:$O$16</c:f>
+              <c:f>'Sprint 2'!$E$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>87.0</c:v>
+                  <c:v>84.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,7 +1486,7 @@
           <c:order val="1"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$E$17:$O$17</c:f>
+              <c:f>'Sprint 2'!$E$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1591,13 +1662,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1765300</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1907,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E37" sqref="B37:E37"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4355,43 +4426,43 @@
         <v>254</v>
       </c>
       <c r="G38" s="4">
-        <f t="shared" ref="F38:P38" si="0">SUM(G5:G36)</f>
+        <f>SUM(G5:G36)</f>
         <v>239</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(H5:H36)</f>
         <v>226</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(I5:I36)</f>
         <v>205</v>
       </c>
       <c r="J38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(J5:J36)</f>
         <v>205</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(K5:K36)</f>
         <v>167</v>
       </c>
       <c r="L38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(L5:L36)</f>
         <v>152</v>
       </c>
       <c r="M38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(M5:M36)</f>
         <v>111</v>
       </c>
       <c r="N38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(N5:N36)</f>
         <v>95</v>
       </c>
       <c r="O38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(O5:O36)</f>
         <v>92</v>
       </c>
       <c r="P38" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(P5:P36)</f>
         <v>72</v>
       </c>
       <c r="Q38" s="4">
@@ -4422,67 +4493,67 @@
         <v>240</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" ref="G39:L39" si="1">F39-15</f>
+        <f t="shared" ref="G39:L39" si="0">F39-15</f>
         <v>225</v>
       </c>
       <c r="H39" s="4">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="J39" s="4">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="K39" s="4">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="L39" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="M39" s="4">
+        <f t="shared" ref="M39:V39" si="1">L39-15</f>
+        <v>135</v>
+      </c>
+      <c r="N39" s="4">
         <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="I39" s="4">
+        <v>120</v>
+      </c>
+      <c r="O39" s="4">
         <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-      <c r="J39" s="4">
+        <v>105</v>
+      </c>
+      <c r="P39" s="4">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="K39" s="4">
+        <v>90</v>
+      </c>
+      <c r="Q39" s="4">
         <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-      <c r="L39" s="4">
+        <v>75</v>
+      </c>
+      <c r="R39" s="4">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="M39" s="4">
-        <f t="shared" ref="M39:V39" si="2">L39-15</f>
-        <v>135</v>
-      </c>
-      <c r="N39" s="4">
-        <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="O39" s="4">
-        <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-      <c r="P39" s="4">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="Q39" s="4">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="R39" s="4">
-        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="S39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="T39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="V39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W39" s="4"/>
@@ -5311,7 +5382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -6441,15 +6512,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6847,27 +6918,27 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" ht="15" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E15" s="4">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F15" s="4">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G15" s="4">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -6879,23 +6950,26 @@
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="35"/>
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="E16" s="4">
-        <f>SUM(E3:E15)</f>
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
-        <f>SUM(F3:F15)</f>
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="G16" s="4">
-        <f>G15</f>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -6907,54 +6981,190 @@
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="4">
+        <f>SUM(E3:E20)</f>
+        <v>84</v>
+      </c>
+      <c r="F21" s="4">
+        <f>SUM(F14:F20)</f>
+        <v>27</v>
+      </c>
+      <c r="G21" s="4">
+        <f>SUM(G15:G20)</f>
+        <v>12</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="4">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="4">
         <v>120</v>
       </c>
-      <c r="F17" s="4">
-        <f t="shared" ref="F17:M17" si="0">E17-15</f>
+      <c r="F22" s="4">
+        <f t="shared" ref="F22:M22" si="0">E22-15</f>
         <v>105</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H22" s="4">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I22" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J22" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L22" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M22" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added a User for floggit in DB and changed the user info in java class DB info
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="3"/>
+    <workbookView xWindow="780" yWindow="320" windowWidth="25600" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ADI-burndown" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="152">
   <si>
     <t>Project</t>
   </si>
@@ -457,6 +457,36 @@
   </si>
   <si>
     <t xml:space="preserve">Ändra Product API </t>
+  </si>
+  <si>
+    <t>Testa</t>
+  </si>
+  <si>
+    <t>KFUAAA</t>
+  </si>
+  <si>
+    <t>Task 6.1</t>
+  </si>
+  <si>
+    <t>Task 6.2</t>
+  </si>
+  <si>
+    <t>Task 6.3</t>
+  </si>
+  <si>
+    <t>Task 6.4</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Log4J</t>
+  </si>
+  <si>
+    <t>Junit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrum Agile XP </t>
   </si>
 </sst>
 </file>
@@ -787,7 +817,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -808,6 +838,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -954,7 +992,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1006,6 +1044,10 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
@@ -1037,6 +1079,10 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1202,11 +1248,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099805528"/>
-        <c:axId val="2099808504"/>
+        <c:axId val="2124952376"/>
+        <c:axId val="2124955352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099805528"/>
+        <c:axId val="2124952376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099808504"/>
+        <c:crossAx val="2124955352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1223,7 +1269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099808504"/>
+        <c:axId val="2124955352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,14 +1280,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099805528"/>
+        <c:crossAx val="2124952376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1384,11 +1429,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099895224"/>
-        <c:axId val="2099898200"/>
+        <c:axId val="2125042168"/>
+        <c:axId val="2125045144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099895224"/>
+        <c:axId val="2125042168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,7 +1442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099898200"/>
+        <c:crossAx val="2125045144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1405,7 +1450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099898200"/>
+        <c:axId val="2125045144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,14 +1461,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099895224"/>
+        <c:crossAx val="2125042168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1463,18 +1507,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$E$21:$O$21</c:f>
+              <c:f>'Sprint 2'!$E$25:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>84.0</c:v>
+                  <c:v>126.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.0</c:v>
+                  <c:v>78.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,7 +1533,7 @@
           <c:order val="1"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$E$22:$O$22</c:f>
+              <c:f>'Sprint 2'!$E$26:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1532,11 +1579,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099934200"/>
-        <c:axId val="2099937176"/>
+        <c:axId val="2125081320"/>
+        <c:axId val="2125084296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099934200"/>
+        <c:axId val="2125081320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +1592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099937176"/>
+        <c:crossAx val="2125084296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +1600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099937176"/>
+        <c:axId val="2125084296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1564,7 +1611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099934200"/>
+        <c:crossAx val="2125081320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1662,13 +1709,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1765300</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4426,43 +4473,43 @@
         <v>254</v>
       </c>
       <c r="G38" s="4">
-        <f>SUM(G5:G36)</f>
+        <f t="shared" ref="G38:P38" si="0">SUM(G5:G36)</f>
         <v>239</v>
       </c>
       <c r="H38" s="4">
-        <f>SUM(H5:H36)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="I38" s="4">
-        <f>SUM(I5:I36)</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
       <c r="J38" s="4">
-        <f>SUM(J5:J36)</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
       <c r="K38" s="4">
-        <f>SUM(K5:K36)</f>
+        <f t="shared" si="0"/>
         <v>167</v>
       </c>
       <c r="L38" s="4">
-        <f>SUM(L5:L36)</f>
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="M38" s="4">
-        <f>SUM(M5:M36)</f>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
       <c r="N38" s="4">
-        <f>SUM(N5:N36)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="O38" s="4">
-        <f>SUM(O5:O36)</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
       <c r="P38" s="4">
-        <f>SUM(P5:P36)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="Q38" s="4">
@@ -4493,67 +4540,67 @@
         <v>240</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" ref="G39:L39" si="0">F39-15</f>
+        <f t="shared" ref="G39:L39" si="1">F39-15</f>
         <v>225</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>165</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" ref="M39:V39" si="1">L39-15</f>
+        <f t="shared" ref="M39:V39" si="2">L39-15</f>
         <v>135</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="O39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="P39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="Q39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="R39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="S39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="T39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="V39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W39" s="4"/>
@@ -4935,7 +4982,6 @@
     <mergeCell ref="B39:D39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6512,10 +6558,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6606,9 +6652,15 @@
       <c r="E3" s="4">
         <v>15</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -6636,8 +6688,12 @@
       <c r="F4" s="4">
         <v>9</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -6662,9 +6718,15 @@
       <c r="E5" s="4">
         <v>9</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -6689,9 +6751,15 @@
       <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -6716,9 +6784,15 @@
       <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -6743,9 +6817,15 @@
       <c r="E8" s="4">
         <v>3</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -6770,9 +6850,15 @@
       <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -6797,9 +6883,15 @@
       <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -6824,9 +6916,15 @@
       <c r="E11" s="4">
         <v>3</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -6851,9 +6949,15 @@
       <c r="E12" s="4">
         <v>3</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -6878,9 +6982,15 @@
       <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -6908,8 +7018,12 @@
       <c r="F14" s="4">
         <v>15</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -6940,7 +7054,9 @@
       <c r="G15" s="4">
         <v>6</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -6971,7 +7087,9 @@
       <c r="G16" s="4">
         <v>2</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -7002,7 +7120,9 @@
       <c r="G17" s="4">
         <v>2</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -7033,7 +7153,9 @@
       <c r="G18" s="4">
         <v>2</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -7052,11 +7174,21 @@
       <c r="C19" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4">
+        <v>6</v>
+      </c>
+      <c r="G19" s="4">
+        <v>6</v>
+      </c>
+      <c r="H19" s="4">
+        <v>6</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -7089,25 +7221,30 @@
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="E21" s="4">
-        <f>SUM(E3:E20)</f>
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F21" s="4">
-        <f>SUM(F14:F20)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G21" s="4">
-        <f>SUM(G15:G20)</f>
-        <v>12</v>
-      </c>
-      <c r="H21" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="H21" s="4">
+        <v>9</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -7117,54 +7254,184 @@
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="4">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4">
+        <v>9</v>
+      </c>
+      <c r="G22" s="4">
+        <v>9</v>
+      </c>
+      <c r="H22" s="4">
+        <v>9</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="4">
+        <v>9</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9</v>
+      </c>
+      <c r="G23" s="4">
+        <v>9</v>
+      </c>
+      <c r="H23" s="4">
+        <v>9</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="4">
+        <v>9</v>
+      </c>
+      <c r="F24" s="4">
+        <v>9</v>
+      </c>
+      <c r="G24" s="4">
+        <v>9</v>
+      </c>
+      <c r="H24" s="4">
+        <v>9</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="4">
+        <f>SUM(E3:E24)</f>
+        <v>126</v>
+      </c>
+      <c r="F25" s="4">
+        <f>SUM(F3:F24)</f>
+        <v>78</v>
+      </c>
+      <c r="G25" s="4">
+        <f>SUM(G3:G24)</f>
+        <v>54</v>
+      </c>
+      <c r="H25" s="4">
+        <f>SUM(H10:H24)</f>
+        <v>42</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="4">
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="4">
         <v>120</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" ref="F22:M22" si="0">E22-15</f>
+      <c r="F26" s="4">
+        <f t="shared" ref="F26:M26" si="0">E26-15</f>
         <v>105</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H26" s="4">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I26" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J26" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K26" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L26" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M26" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Deleted som .pdf files
</commit_message>
<xml_diff>
--- a/ADI-scrum-BrndownChart.xlsx
+++ b/ADI-scrum-BrndownChart.xlsx
@@ -712,15 +712,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -951,11 +951,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090752696"/>
-        <c:axId val="2090755672"/>
+        <c:axId val="2030090344"/>
+        <c:axId val="2030087352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090752696"/>
+        <c:axId val="2030090344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090755672"/>
+        <c:crossAx val="2030087352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -972,7 +972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090755672"/>
+        <c:axId val="2030087352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090752696"/>
+        <c:crossAx val="2030090344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1111,11 +1111,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090791976"/>
-        <c:axId val="2090794952"/>
+        <c:axId val="2074436104"/>
+        <c:axId val="2074439080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090791976"/>
+        <c:axId val="2074436104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,7 +1124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090794952"/>
+        <c:crossAx val="2074439080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1132,7 +1132,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090794952"/>
+        <c:axId val="2074439080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090791976"/>
+        <c:crossAx val="2074436104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2539,11 +2539,11 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="11"/>
       <c r="E23" s="4">
         <f t="shared" ref="E23:O23" si="0">SUM(E3:E22)</f>
@@ -2591,11 +2591,11 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="11"/>
       <c r="E24" s="4">
         <v>120</v>
@@ -2654,7 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -3550,11 +3550,11 @@
       <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="11"/>
       <c r="E24" s="4">
         <f>SUM(E3:E23)</f>
@@ -3590,11 +3590,11 @@
       <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="11"/>
       <c r="E25" s="4">
         <v>120</v>
@@ -3654,7 +3654,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3665,91 +3665,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="165">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="60">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" ht="45">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>